<commit_message>
First draft of pipeline for categorical factors
</commit_message>
<xml_diff>
--- a/full_fact.xlsx
+++ b/full_fact.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive - epfl.ch\Desktop\EPFL PhD\ENG 606a DOE\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyrilmonette/Desktop/EPFL 2018-2026/PhD - Mobots/ENG-606/project/RoboticFrameCharacterisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE825DA8-D1B1-484A-AEB5-E916A14DF103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16A891B-8281-064B-8A6E-4DD7BBBA9692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="31940" windowHeight="18160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="full_fact" sheetId="1" r:id="rId1"/>
@@ -982,18 +982,18 @@
   <dimension ref="A1:AG55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="12" max="12" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.7265625" style="1"/>
-    <col min="24" max="24" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" style="1"/>
+    <col min="24" max="24" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>3.0833333333333299</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>3.4166666666666652</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>3.4166666666666599</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>2.3333333333333299</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>1.9999999999999951</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>1.9166666666666601</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>2.2916666666666652</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>1.9166666666666601</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>3.6666666666666599</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>3.4166666666666599</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>2.6249999999999947</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>2.1666666666666599</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>2.3333333333333299</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>2.6249999999999947</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>2.3333333333333299</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>1.5833333333333299</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>1.9166666666666601</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>3.0833333333333299</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>3.4166666666666599</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>3.5833333333333299</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>3.0833333333333299</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>3.4166666666666599</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>2.3333333333333299</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>3.0833333333333299</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>2.0833333333333299</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>1.9166666666666601</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>1.9166666666666601</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>1.9166666666666601</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>9</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>9</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>2.9166666666666652</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>9</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>1.791666666666665</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>9</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>2.6249999999999951</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>9</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>1.916666666666665</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>9</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>2.4583333333333299</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>14</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>3.2083333333333299</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>14</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>3.5416666666666599</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>14</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>3.3333333333333299</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>14</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>3.4583333333333299</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>14</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>3.1666666666666652</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>14</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>3.4583333333333299</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>15</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>2.3333333333333299</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>15</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>2.9999999999999947</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>15</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>2.3333333333333299</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>15</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>2.0416666666666599</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>15</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>2.1249999999999951</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>15</v>
       </c>

</xml_diff>